<commit_message>
PO Test Case Migration
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/POLoader_AutomationOrg.xlsx
+++ b/templates/AutomationOrg/POLoader_AutomationOrg.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dellDevonforce\Provar\ErpFinalProject\rsqasampleproj\rsqasampleproj\templates\AutomationOrg\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Namrata\git\rsqasampleproj\templates\AutomationOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64EB850A-0C59-48B2-97FC-2E0537E80BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3274D562-EB22-4AA6-A42A-462E2F194FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{B6C21A89-21B4-4624-A955-66D166717697}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="4" xr2:uid="{B6C21A89-21B4-4624-A955-66D166717697}"/>
   </bookViews>
   <sheets>
     <sheet name="AddBoth" sheetId="15" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="48">
   <si>
     <t>Vendor</t>
   </si>
@@ -90,12 +90,6 @@
     <t>Unit Price</t>
   </si>
   <si>
-    <t>Dim1</t>
-  </si>
-  <si>
-    <t>Dim4</t>
-  </si>
-  <si>
     <t>Add Both</t>
   </si>
   <si>
@@ -114,18 +108,6 @@
     <t>India</t>
   </si>
   <si>
-    <t>TEST1</t>
-  </si>
-  <si>
-    <t>Distributor</t>
-  </si>
-  <si>
-    <t>Blue Widgets</t>
-  </si>
-  <si>
-    <t>Dim2</t>
-  </si>
-  <si>
     <t>Process</t>
   </si>
   <si>
@@ -171,9 +153,6 @@
     <t>NP_Automation</t>
   </si>
   <si>
-    <t>a351K000001fwBg</t>
-  </si>
-  <si>
     <t>Icitem</t>
   </si>
   <si>
@@ -199,6 +178,15 @@
   </si>
   <si>
     <t>a415f000000lOCE</t>
+  </si>
+  <si>
+    <t>a415f000000lOC9</t>
+  </si>
+  <si>
+    <t>a415f000000lOCn</t>
+  </si>
+  <si>
+    <t>a415f000000lOCi</t>
   </si>
 </sst>
 </file>
@@ -557,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D721CDB-A9DB-40A7-92FA-BE728EC43FA8}">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C5"/>
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,18 +559,18 @@
     <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
         <v>6</v>
@@ -620,19 +608,10 @@
       <c r="P1" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" t="s">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>15</v>
-      </c>
-      <c r="R1" t="s">
-        <v>26</v>
-      </c>
-      <c r="S1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>17</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -641,34 +620,34 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
         <v>18</v>
       </c>
-      <c r="F2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>19</v>
-      </c>
-      <c r="I2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" t="s">
-        <v>21</v>
       </c>
       <c r="K2">
         <v>411002</v>
       </c>
       <c r="L2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="N2">
         <v>4</v>
@@ -677,57 +656,48 @@
         <v>200.55</v>
       </c>
       <c r="P2" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>23</v>
-      </c>
-      <c r="R2" t="s">
-        <v>24</v>
-      </c>
-      <c r="S2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="I3" t="s">
         <v>18</v>
       </c>
-      <c r="F3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>19</v>
-      </c>
-      <c r="I3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" t="s">
-        <v>21</v>
       </c>
       <c r="K3">
         <v>411002</v>
       </c>
       <c r="L3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="N3">
         <v>4</v>
@@ -736,21 +706,12 @@
         <v>200.55</v>
       </c>
       <c r="P3" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>23</v>
-      </c>
-      <c r="R3" t="s">
-        <v>24</v>
-      </c>
-      <c r="S3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
@@ -759,34 +720,34 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" t="s">
         <v>18</v>
       </c>
-      <c r="F4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>19</v>
-      </c>
-      <c r="I4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" t="s">
-        <v>21</v>
       </c>
       <c r="K4">
         <v>411002</v>
       </c>
       <c r="L4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="N4">
         <v>4</v>
@@ -795,57 +756,48 @@
         <v>200.55</v>
       </c>
       <c r="P4" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>23</v>
-      </c>
-      <c r="R4" t="s">
-        <v>24</v>
-      </c>
-      <c r="S4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="b">
-        <v>0</v>
-      </c>
-      <c r="C5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="I5" t="s">
         <v>18</v>
       </c>
-      <c r="F5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G5" t="s">
-        <v>48</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>19</v>
-      </c>
-      <c r="I5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" t="s">
-        <v>21</v>
       </c>
       <c r="K5">
         <v>411002</v>
       </c>
       <c r="L5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="N5">
         <v>4</v>
@@ -854,16 +806,7 @@
         <v>200.55</v>
       </c>
       <c r="P5" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>23</v>
-      </c>
-      <c r="R5" t="s">
-        <v>24</v>
-      </c>
-      <c r="S5" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -874,27 +817,23 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAC89EBC-4F44-4337-884E-CD4887F2A248}">
-  <dimension ref="A1:T5"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E5"/>
+      <selection activeCell="I12" sqref="H12:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.28515625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
@@ -909,51 +848,36 @@
         <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
         <v>2</v>
       </c>
-      <c r="R1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" t="s">
-        <v>26</v>
-      </c>
-      <c r="T1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -965,235 +889,81 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
         <v>18</v>
       </c>
-      <c r="G2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>19</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2">
+        <v>411002</v>
+      </c>
+      <c r="L2" t="s">
         <v>20</v>
       </c>
-      <c r="K2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2">
+      <c r="M2">
+        <v>5</v>
+      </c>
+      <c r="N2">
+        <v>1500</v>
+      </c>
+      <c r="O2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3">
         <v>411002</v>
       </c>
-      <c r="M2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="O2">
-        <v>5</v>
-      </c>
-      <c r="P2">
-        <v>1500</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>49</v>
-      </c>
-      <c r="R2" t="s">
-        <v>23</v>
-      </c>
-      <c r="S2" t="s">
-        <v>24</v>
-      </c>
-      <c r="T2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H3" t="s">
-        <v>47</v>
-      </c>
-      <c r="I3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>20</v>
       </c>
-      <c r="K3" t="s">
-        <v>21</v>
-      </c>
-      <c r="L3">
-        <v>411002</v>
-      </c>
-      <c r="M3" t="s">
-        <v>22</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="O3">
+      <c r="M3">
         <v>10</v>
       </c>
-      <c r="P3">
+      <c r="N3">
         <v>2460</v>
       </c>
-      <c r="Q3" t="s">
-        <v>49</v>
-      </c>
-      <c r="R3" t="s">
-        <v>23</v>
-      </c>
-      <c r="S3" t="s">
-        <v>24</v>
-      </c>
-      <c r="T3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" t="b">
-        <v>0</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H4" t="s">
-        <v>48</v>
-      </c>
-      <c r="I4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" t="s">
-        <v>21</v>
-      </c>
-      <c r="L4">
-        <v>411002</v>
-      </c>
-      <c r="M4" t="s">
-        <v>22</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="O4">
-        <v>5</v>
-      </c>
-      <c r="P4">
-        <v>1500</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>49</v>
-      </c>
-      <c r="R4" t="s">
-        <v>23</v>
-      </c>
-      <c r="S4" t="s">
-        <v>24</v>
-      </c>
-      <c r="T4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" t="s">
-        <v>46</v>
-      </c>
-      <c r="H5" t="s">
-        <v>48</v>
-      </c>
-      <c r="I5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" t="s">
-        <v>20</v>
-      </c>
-      <c r="K5" t="s">
-        <v>21</v>
-      </c>
-      <c r="L5">
-        <v>411002</v>
-      </c>
-      <c r="M5" t="s">
-        <v>22</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="O5">
-        <v>10</v>
-      </c>
-      <c r="P5">
-        <v>2460</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>49</v>
-      </c>
-      <c r="R5" t="s">
-        <v>23</v>
-      </c>
-      <c r="S5" t="s">
-        <v>24</v>
-      </c>
-      <c r="T5" t="s">
-        <v>25</v>
+      <c r="O3" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1206,7 +976,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G3"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1228,10 +998,10 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
         <v>6</v>
@@ -1257,66 +1027,66 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2" t="b">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="F2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="H2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I2">
-        <v>200.55</v>
+        <v>450</v>
       </c>
       <c r="J2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="F3" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="H3">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I3">
-        <v>200.55</v>
+        <v>300</v>
       </c>
       <c r="J3" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1328,8 +1098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA76DEB8-C288-4FFF-933C-5D83C119E0BF}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1341,7 +1111,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
@@ -1355,30 +1125,30 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1410,36 +1180,36 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E2">
         <v>10</v>
@@ -1448,10 +1218,10 @@
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="H2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1463,8 +1233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D68A558F-1570-4CED-A748-7B569825A34D}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1481,16 +1251,16 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -1498,16 +1268,16 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" t="s">
-        <v>42</v>
+        <v>22</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="E2">
         <v>10</v>
@@ -1516,21 +1286,21 @@
         <v>15.897</v>
       </c>
       <c r="G2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" t="s">
-        <v>42</v>
+        <v>22</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="E3">
         <v>10</v>
@@ -1539,7 +1309,7 @@
         <v>15.897</v>
       </c>
       <c r="G3" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1549,10 +1319,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{683E8783-6B26-40B7-87D9-A6B8B4FD7B23}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D5" sqref="D5:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1568,16 +1338,16 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -1585,48 +1355,117 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E2">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F2">
-        <v>10</v>
+        <v>33.768000000000001</v>
       </c>
       <c r="G2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E3">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="F3">
+        <v>44</v>
+      </c>
+      <c r="G3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
         <v>100</v>
       </c>
-      <c r="G3" t="s">
-        <v>49</v>
+      <c r="G4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>340</v>
+      </c>
+      <c r="G5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>22.69</v>
+      </c>
+      <c r="G6" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1639,7 +1478,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F5"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1653,10 +1492,10 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
         <v>6</v>
@@ -1683,42 +1522,42 @@
         <v>12</v>
       </c>
       <c r="L1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" t="s">
         <v>28</v>
       </c>
-      <c r="D2" t="s">
+      <c r="H2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" t="s">
-        <v>20</v>
-      </c>
       <c r="I2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J2">
         <v>411011</v>
       </c>
       <c r="K2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L2" t="b">
         <v>1</v>
@@ -1726,37 +1565,37 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" t="s">
-        <v>20</v>
-      </c>
       <c r="I3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J3">
         <v>411018</v>
       </c>
       <c r="K3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L3" t="b">
         <v>0</v>
@@ -1764,37 +1603,37 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
       </c>
       <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" t="s">
         <v>28</v>
       </c>
-      <c r="D4" t="s">
+      <c r="H4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" t="s">
-        <v>20</v>
-      </c>
       <c r="I4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J4">
         <v>411011</v>
       </c>
       <c r="K4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L4" t="b">
         <v>1</v>
@@ -1802,37 +1641,37 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B5" t="b">
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" t="s">
-        <v>20</v>
-      </c>
       <c r="I5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J5">
         <v>411018</v>
       </c>
       <c r="K5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L5" t="b">
         <v>0</v>
@@ -1845,10 +1684,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BAAF839-3C85-47A3-8C0F-A4F8E32EA17E}">
-  <dimension ref="A1:T5"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1856,19 +1695,18 @@
     <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
@@ -1883,51 +1721,39 @@
         <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M1" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="N1" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
         <v>2</v>
       </c>
-      <c r="R1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" t="s">
-        <v>26</v>
-      </c>
-      <c r="T1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -1939,57 +1765,45 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="H2" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="I2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="J2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2">
+        <v>19</v>
+      </c>
+      <c r="K2">
         <v>400056</v>
       </c>
-      <c r="M2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>50</v>
+      <c r="L2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N2">
+        <v>10</v>
       </c>
       <c r="O2">
         <v>10</v>
       </c>
-      <c r="P2">
-        <v>10</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>49</v>
-      </c>
-      <c r="R2" t="s">
-        <v>23</v>
-      </c>
-      <c r="S2" t="s">
-        <v>24</v>
-      </c>
-      <c r="T2" t="s">
+      <c r="P2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>31</v>
-      </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
@@ -2001,173 +1815,37 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" t="s">
         <v>18</v>
       </c>
-      <c r="G3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H3" t="s">
-        <v>47</v>
-      </c>
-      <c r="I3" t="s">
-        <v>38</v>
-      </c>
       <c r="J3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3">
+        <v>400056</v>
+      </c>
+      <c r="L3" t="s">
         <v>20</v>
       </c>
-      <c r="K3" t="s">
-        <v>21</v>
-      </c>
-      <c r="L3">
-        <v>400056</v>
-      </c>
-      <c r="M3" t="s">
-        <v>22</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>50</v>
+      <c r="M3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N3">
+        <v>6</v>
       </c>
       <c r="O3">
-        <v>6</v>
-      </c>
-      <c r="P3">
         <v>1000</v>
       </c>
-      <c r="Q3" t="s">
-        <v>49</v>
-      </c>
-      <c r="R3" t="s">
-        <v>23</v>
-      </c>
-      <c r="S3" t="s">
-        <v>24</v>
-      </c>
-      <c r="T3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" t="b">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H4" t="s">
-        <v>48</v>
-      </c>
-      <c r="I4" t="s">
-        <v>36</v>
-      </c>
-      <c r="J4" t="s">
-        <v>37</v>
-      </c>
-      <c r="K4" t="s">
-        <v>21</v>
-      </c>
-      <c r="L4">
-        <v>400056</v>
-      </c>
-      <c r="M4" t="s">
-        <v>22</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="O4">
-        <v>10</v>
-      </c>
-      <c r="P4">
-        <v>10</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>49</v>
-      </c>
-      <c r="R4" t="s">
-        <v>23</v>
-      </c>
-      <c r="S4" t="s">
-        <v>24</v>
-      </c>
-      <c r="T4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" t="s">
-        <v>46</v>
-      </c>
-      <c r="H5" t="s">
-        <v>48</v>
-      </c>
-      <c r="I5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J5" t="s">
-        <v>20</v>
-      </c>
-      <c r="K5" t="s">
-        <v>21</v>
-      </c>
-      <c r="L5">
-        <v>400056</v>
-      </c>
-      <c r="M5" t="s">
-        <v>22</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="O5">
-        <v>6</v>
-      </c>
-      <c r="P5">
-        <v>1000</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>49</v>
-      </c>
-      <c r="R5" t="s">
-        <v>23</v>
-      </c>
-      <c r="S5" t="s">
-        <v>24</v>
-      </c>
-      <c r="T5" t="s">
-        <v>25</v>
+      <c r="P3" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -2177,27 +1855,27 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69D1DF1B-CADC-480B-9F9D-24CB1D04E075}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D5"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
@@ -2209,33 +1887,21 @@
         <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" t="s">
         <v>2</v>
       </c>
-      <c r="K1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>26</v>
       </c>
-      <c r="M1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>32</v>
-      </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -2244,39 +1910,27 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G2" t="s">
-        <v>47</v>
+        <v>39</v>
+      </c>
+      <c r="G2">
+        <v>6</v>
       </c>
       <c r="H2">
-        <v>6</v>
-      </c>
-      <c r="I2">
         <v>2000</v>
       </c>
-      <c r="J2" t="s">
-        <v>49</v>
-      </c>
-      <c r="K2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
@@ -2285,113 +1939,19 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3" t="s">
-        <v>47</v>
+        <v>39</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
       </c>
       <c r="H3">
-        <v>3</v>
-      </c>
-      <c r="I3">
         <v>250</v>
       </c>
-      <c r="J3" t="s">
-        <v>49</v>
-      </c>
-      <c r="K3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4">
-        <v>6</v>
-      </c>
-      <c r="I4">
-        <v>2000</v>
-      </c>
-      <c r="J4" t="s">
-        <v>49</v>
-      </c>
-      <c r="K4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L4" t="s">
-        <v>24</v>
-      </c>
-      <c r="M4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G5" t="s">
-        <v>48</v>
-      </c>
-      <c r="H5">
-        <v>3</v>
-      </c>
-      <c r="I5">
-        <v>250</v>
-      </c>
-      <c r="J5" t="s">
-        <v>49</v>
-      </c>
-      <c r="K5" t="s">
-        <v>23</v>
-      </c>
-      <c r="L5" t="s">
-        <v>24</v>
-      </c>
-      <c r="M5" t="s">
-        <v>25</v>
+      <c r="I3" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>